<commit_message>
updated script with multiple dates checking
</commit_message>
<xml_diff>
--- a/source-master-v2.xlsx
+++ b/source-master-v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\Documents\DigitalDi\Python Shiv\mohan_script\mohan_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D9D225-616C-4064-96AF-0D4D5E74D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55577234-A741-442D-9E2E-997441C372FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D32566AC-B4DA-41DD-9D43-E8DE8046892B}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="835">
   <si>
     <t>Subject</t>
   </si>
@@ -4604,9 +4604,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4644,7 +4644,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4750,7 +4750,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4892,7 +4892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4902,8 +4902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051B4B0B-A9E8-4734-82AB-B1D62151FB8E}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4996,6 +4996,9 @@
       </c>
       <c r="L2" t="s">
         <v>824</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>